<commit_message>
more complicated MTM table
</commit_message>
<xml_diff>
--- a/data1.xlsx
+++ b/data1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yuyulu\Documents\thesis\HRC_taskAlloc_w.TB_w.AR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B1A1D0B-0664-4478-B558-3FBCC01995F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB3CFF9-C73D-4585-81A8-62217928FC9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16080" yWindow="8130" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Position" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,23 @@
     <sheet name="Therbligs(L)" sheetId="3" r:id="rId3"/>
     <sheet name="Therbligs(R)" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="26">
   <si>
     <t>Type</t>
   </si>
@@ -40,9 +51,6 @@
     <t>Obj2</t>
   </si>
   <si>
-    <t>TE</t>
-  </si>
-  <si>
     <t>R</t>
   </si>
   <si>
@@ -61,9 +69,6 @@
     <t>Stuff</t>
   </si>
   <si>
-    <t>TL</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -89,6 +94,30 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>R</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RL</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Type</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -144,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -174,6 +203,9 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -494,21 +526,21 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B2" s="8">
         <v>-0.2</v>
@@ -522,7 +554,7 @@
     </row>
     <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="8">
         <v>0.2</v>
@@ -536,7 +568,7 @@
     </row>
     <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B4" s="9">
         <v>0</v>
@@ -550,7 +582,7 @@
     </row>
     <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="8">
         <v>-0.3</v>
@@ -564,7 +596,7 @@
     </row>
     <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="8">
         <v>-0.2</v>
@@ -578,7 +610,7 @@
     </row>
     <row r="7" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B7" s="8">
         <v>0.3</v>
@@ -613,12 +645,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -638,10 +670,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -650,7 +682,7 @@
     <col min="2" max="5" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -660,14 +692,17 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
     </row>
   </sheetData>
@@ -683,17 +718,17 @@
   </sheetPr>
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="13.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="10" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="13.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="6.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
@@ -701,7 +736,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -709,13 +744,15 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -727,15 +764,17 @@
     </row>
     <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -749,14 +788,13 @@
     </row>
     <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -769,17 +807,16 @@
     </row>
     <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -791,14 +828,13 @@
     </row>
     <row r="5" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -811,15 +847,17 @@
     </row>
     <row r="6" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="C6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -833,14 +871,13 @@
     </row>
     <row r="7" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -853,15 +890,17 @@
     </row>
     <row r="8" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -875,14 +914,13 @@
     </row>
     <row r="9" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
-      <c r="D9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -895,15 +933,17 @@
     </row>
     <row r="10" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="C10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -917,14 +957,13 @@
     </row>
     <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -937,17 +976,16 @@
     </row>
     <row r="12" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="E12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -959,14 +997,13 @@
     </row>
     <row r="13" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
-      <c r="D13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -979,15 +1016,17 @@
     </row>
     <row r="14" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="C14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -1001,14 +1040,13 @@
     </row>
     <row r="15" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
-      <c r="D15" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="2"/>
+      <c r="E15" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -1021,17 +1059,16 @@
     </row>
     <row r="16" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
-      <c r="D16" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="E16" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -1043,14 +1080,13 @@
     </row>
     <row r="17" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
-      <c r="D17" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -1063,15 +1099,17 @@
     </row>
     <row r="18" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="C18" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -1085,14 +1123,13 @@
     </row>
     <row r="19" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
-      <c r="D19" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="2"/>
+      <c r="E19" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
@@ -1105,15 +1142,17 @@
     </row>
     <row r="20" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -1127,14 +1166,13 @@
     </row>
     <row r="21" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
-      <c r="D21" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="2"/>
+      <c r="E21" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -1147,15 +1185,17 @@
     </row>
     <row r="22" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="C22" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
@@ -1169,14 +1209,13 @@
     </row>
     <row r="23" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
-      <c r="D23" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23" s="2"/>
+      <c r="E23" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
@@ -1189,15 +1228,17 @@
     </row>
     <row r="24" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -1211,14 +1252,13 @@
     </row>
     <row r="25" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
-      <c r="D25" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25" s="2"/>
+      <c r="E25" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
@@ -1231,15 +1271,17 @@
     </row>
     <row r="26" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="C26" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
@@ -1253,14 +1295,13 @@
     </row>
     <row r="27" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" s="2"/>
+      <c r="E27" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -1273,17 +1314,16 @@
     </row>
     <row r="28" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="E28" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F28" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
@@ -1295,14 +1335,13 @@
     </row>
     <row r="29" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E29" s="2"/>
+      <c r="E29" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>

</xml_diff>